<commit_message>
convert subject names in excel to lowercase to reduce chance of mismatch with dict
</commit_message>
<xml_diff>
--- a/Sample input.xlsx
+++ b/Sample input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Coding\PredictedGradeFlask\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF03A54D-0EA8-4807-B5D3-67777B5AF253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89EF8B0-8FD0-41A2-9A67-1F3573ED2F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1731" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1731" uniqueCount="199">
   <si>
     <t>Progression 1 Marks out of 100</t>
   </si>
@@ -439,22 +439,13 @@
     <t xml:space="preserve">Biology  </t>
   </si>
   <si>
-    <t xml:space="preserve">Pyschology </t>
-  </si>
-  <si>
     <t xml:space="preserve">Physics </t>
   </si>
   <si>
     <t xml:space="preserve">Math AA </t>
   </si>
   <si>
-    <t xml:space="preserve">English SL </t>
-  </si>
-  <si>
     <t>French AB</t>
-  </si>
-  <si>
-    <t>spanish B</t>
   </si>
   <si>
     <t xml:space="preserve">Chemistry </t>
@@ -467,12 +458,6 @@
   </si>
   <si>
     <t>ab</t>
-  </si>
-  <si>
-    <t>French ab</t>
-  </si>
-  <si>
-    <t>Math AI SL</t>
   </si>
   <si>
     <t xml:space="preserve">English </t>
@@ -1455,24 +1440,6 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="4" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1494,6 +1461,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1803,8 +1788,8 @@
   <dimension ref="A1:AA1200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1121" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1144" sqref="B1144"/>
+      <pane ySplit="1" topLeftCell="A800" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I808" sqref="I808"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1851,13 +1836,13 @@
       <c r="H1" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="I1" s="146"/>
-      <c r="J1" s="147"/>
-      <c r="K1" s="147"/>
-      <c r="L1" s="147"/>
-      <c r="M1" s="148"/>
-      <c r="N1" s="148"/>
-      <c r="O1" s="143"/>
+      <c r="I1" s="140"/>
+      <c r="J1" s="141"/>
+      <c r="K1" s="141"/>
+      <c r="L1" s="141"/>
+      <c r="M1" s="142"/>
+      <c r="N1" s="142"/>
+      <c r="O1" s="137"/>
       <c r="S1" s="72"/>
     </row>
     <row r="2" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1880,16 +1865,16 @@
       <c r="G2" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="142" t="s">
+      <c r="H2" s="136" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="146"/>
-      <c r="J2" s="147"/>
-      <c r="K2" s="147"/>
-      <c r="L2" s="147"/>
-      <c r="M2" s="147"/>
-      <c r="N2" s="147"/>
-      <c r="O2" s="144"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="141"/>
+      <c r="K2" s="141"/>
+      <c r="L2" s="141"/>
+      <c r="M2" s="141"/>
+      <c r="N2" s="141"/>
+      <c r="O2" s="138"/>
       <c r="P2" s="76"/>
       <c r="Q2" s="76"/>
       <c r="R2" s="76"/>
@@ -1928,13 +1913,13 @@
       <c r="H3" s="80">
         <v>80</v>
       </c>
-      <c r="I3" s="146"/>
-      <c r="J3" s="147"/>
-      <c r="K3" s="147"/>
-      <c r="L3" s="147"/>
-      <c r="M3" s="149"/>
-      <c r="N3" s="149"/>
-      <c r="O3" s="145"/>
+      <c r="I3" s="140"/>
+      <c r="J3" s="141"/>
+      <c r="K3" s="141"/>
+      <c r="L3" s="141"/>
+      <c r="M3" s="143"/>
+      <c r="N3" s="143"/>
+      <c r="O3" s="139"/>
       <c r="P3" s="41"/>
       <c r="Q3" s="41"/>
       <c r="R3" s="41"/>
@@ -1973,13 +1958,13 @@
       <c r="H4" s="80">
         <v>68</v>
       </c>
-      <c r="I4" s="146"/>
-      <c r="J4" s="147"/>
-      <c r="K4" s="147"/>
-      <c r="L4" s="147"/>
-      <c r="M4" s="148"/>
-      <c r="N4" s="148"/>
-      <c r="O4" s="143"/>
+      <c r="I4" s="140"/>
+      <c r="J4" s="141"/>
+      <c r="K4" s="141"/>
+      <c r="L4" s="141"/>
+      <c r="M4" s="142"/>
+      <c r="N4" s="142"/>
+      <c r="O4" s="137"/>
       <c r="S4" s="72"/>
     </row>
     <row r="5" spans="1:27" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2007,13 +1992,13 @@
       <c r="H5" s="80">
         <v>7</v>
       </c>
-      <c r="I5" s="146"/>
-      <c r="J5" s="147"/>
-      <c r="K5" s="147"/>
-      <c r="L5" s="147"/>
-      <c r="M5" s="148"/>
-      <c r="N5" s="148"/>
-      <c r="O5" s="143"/>
+      <c r="I5" s="140"/>
+      <c r="J5" s="141"/>
+      <c r="K5" s="141"/>
+      <c r="L5" s="141"/>
+      <c r="M5" s="142"/>
+      <c r="N5" s="142"/>
+      <c r="O5" s="137"/>
       <c r="S5" s="72"/>
     </row>
     <row r="6" spans="1:27" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2041,13 +2026,13 @@
       <c r="H6" s="80">
         <v>74</v>
       </c>
-      <c r="I6" s="146"/>
-      <c r="J6" s="147"/>
-      <c r="K6" s="147"/>
-      <c r="L6" s="147"/>
-      <c r="M6" s="148"/>
-      <c r="N6" s="148"/>
-      <c r="O6" s="143"/>
+      <c r="I6" s="140"/>
+      <c r="J6" s="141"/>
+      <c r="K6" s="141"/>
+      <c r="L6" s="141"/>
+      <c r="M6" s="142"/>
+      <c r="N6" s="142"/>
+      <c r="O6" s="137"/>
       <c r="S6" s="72"/>
     </row>
     <row r="7" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2079,13 +2064,13 @@
         <f>0.2*H3+0.2*H4+H5+0.5*H6</f>
         <v>73.599999999999994</v>
       </c>
-      <c r="I7" s="146"/>
-      <c r="J7" s="147"/>
-      <c r="K7" s="147"/>
-      <c r="L7" s="147"/>
-      <c r="M7" s="148"/>
-      <c r="N7" s="148"/>
-      <c r="O7" s="143"/>
+      <c r="I7" s="140"/>
+      <c r="J7" s="141"/>
+      <c r="K7" s="141"/>
+      <c r="L7" s="141"/>
+      <c r="M7" s="142"/>
+      <c r="N7" s="142"/>
+      <c r="O7" s="137"/>
       <c r="S7" s="72"/>
     </row>
     <row r="8" spans="1:27" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6243,7 +6228,7 @@
     <row r="155" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="73"/>
       <c r="B155" s="74" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C155" s="75" t="s">
         <v>103</v>
@@ -6726,7 +6711,7 @@
         <v>10494</v>
       </c>
       <c r="B172" s="48" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C172" s="75" t="s">
         <v>12</v>
@@ -7203,7 +7188,7 @@
         <v>12791</v>
       </c>
       <c r="B189" s="48" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C189" s="75" t="s">
         <v>116</v>
@@ -7670,7 +7655,7 @@
     <row r="206" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="73"/>
       <c r="B206" s="48" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C206" s="75" t="s">
         <v>116</v>
@@ -8153,7 +8138,7 @@
     <row r="223" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="73"/>
       <c r="B223" s="48" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C223" s="75" t="s">
         <v>103</v>
@@ -8650,7 +8635,7 @@
         <v>12795</v>
       </c>
       <c r="B240" s="48" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C240" s="75" t="s">
         <v>116</v>
@@ -9125,7 +9110,7 @@
     <row r="257" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="73"/>
       <c r="B257" s="48" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C257" s="75" t="s">
         <v>12</v>
@@ -9600,7 +9585,7 @@
         <v>889</v>
       </c>
       <c r="B274" s="48" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C274" s="75" t="s">
         <v>14</v>
@@ -10082,7 +10067,7 @@
         <v>12799</v>
       </c>
       <c r="B291" s="48" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C291" s="75" t="s">
         <v>116</v>
@@ -10549,7 +10534,7 @@
         <v>12275</v>
       </c>
       <c r="B308" s="48" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C308" s="75" t="s">
         <v>116</v>
@@ -11032,7 +11017,7 @@
         <v>10145</v>
       </c>
       <c r="B325" s="48" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C325" s="75" t="s">
         <v>17</v>
@@ -11521,7 +11506,7 @@
         <v>10149</v>
       </c>
       <c r="B342" s="48" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C342" s="75" t="s">
         <v>12</v>
@@ -12002,7 +11987,7 @@
     <row r="359" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A359" s="73"/>
       <c r="B359" s="48" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C359" s="75" t="s">
         <v>13</v>
@@ -12477,7 +12462,7 @@
         <v>12809</v>
       </c>
       <c r="B376" s="48" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C376" s="75" t="s">
         <v>103</v>
@@ -12962,7 +12947,7 @@
     <row r="393" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A393" s="73"/>
       <c r="B393" s="48" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C393" s="75" t="s">
         <v>131</v>
@@ -13435,7 +13420,7 @@
     <row r="410" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A410" s="73"/>
       <c r="B410" s="48" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C410" s="75" t="s">
         <v>12</v>
@@ -13911,7 +13896,7 @@
         <v>12812</v>
       </c>
       <c r="B427" s="48" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C427" s="75" t="s">
         <v>115</v>
@@ -14396,7 +14381,7 @@
         <v>12813</v>
       </c>
       <c r="B444" s="48" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C444" s="75" t="s">
         <v>115</v>
@@ -14881,7 +14866,7 @@
         <v>12814</v>
       </c>
       <c r="B461" s="48" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C461" s="75" t="s">
         <v>12</v>
@@ -15352,7 +15337,7 @@
         <v>12815</v>
       </c>
       <c r="B478" s="48" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C478" s="75" t="s">
         <v>112</v>
@@ -15370,7 +15355,7 @@
         <v>113</v>
       </c>
       <c r="H478" s="49" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="I478" s="61"/>
       <c r="J478" s="40"/>
@@ -15837,19 +15822,19 @@
         <v>10145</v>
       </c>
       <c r="B495" s="48" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C495" s="75" t="s">
+        <v>132</v>
+      </c>
+      <c r="D495" s="49" t="s">
         <v>133</v>
-      </c>
-      <c r="D495" s="49" t="s">
-        <v>134</v>
       </c>
       <c r="E495" s="49" t="s">
         <v>115</v>
       </c>
       <c r="F495" s="75" t="s">
-        <v>135</v>
+        <v>15</v>
       </c>
       <c r="G495" s="49" t="s">
         <v>113</v>
@@ -16328,7 +16313,7 @@
         <v>12821</v>
       </c>
       <c r="B512" s="48" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C512" s="75" t="s">
         <v>12</v>
@@ -16343,7 +16328,7 @@
         <v>17</v>
       </c>
       <c r="G512" s="49" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H512" s="49" t="s">
         <v>15</v>
@@ -16815,7 +16800,7 @@
     <row r="529" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A529" s="100"/>
       <c r="B529" s="128" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C529" s="101" t="s">
         <v>12</v>
@@ -17285,7 +17270,7 @@
     <row r="546" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A546" s="73"/>
       <c r="B546" s="48" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C546" s="75" t="s">
         <v>12</v>
@@ -17768,7 +17753,7 @@
     <row r="563" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A563" s="73"/>
       <c r="B563" s="48" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C563" s="75" t="s">
         <v>15</v>
@@ -18247,7 +18232,7 @@
     <row r="580" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A580" s="73"/>
       <c r="B580" s="48" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C580" s="75" t="s">
         <v>131</v>
@@ -18724,7 +18709,7 @@
     <row r="597" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A597" s="73"/>
       <c r="B597" s="48" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C597" s="75" t="s">
         <v>110</v>
@@ -19209,7 +19194,7 @@
     <row r="614" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A614" s="73"/>
       <c r="B614" s="48" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C614" s="75" t="s">
         <v>131</v>
@@ -19224,7 +19209,7 @@
         <v>116</v>
       </c>
       <c r="G614" s="49" t="s">
-        <v>137</v>
+        <v>16</v>
       </c>
       <c r="H614" s="49" t="s">
         <v>15</v>
@@ -19684,7 +19669,7 @@
         <v>12837</v>
       </c>
       <c r="B631" s="48" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C631" s="75" t="s">
         <v>115</v>
@@ -19696,7 +19681,7 @@
         <v>103</v>
       </c>
       <c r="F631" s="75" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G631" s="49" t="s">
         <v>113</v>
@@ -20165,7 +20150,7 @@
         <v>12840</v>
       </c>
       <c r="B648" s="48" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C648" s="75" t="s">
         <v>17</v>
@@ -20180,7 +20165,7 @@
         <v>15</v>
       </c>
       <c r="G648" s="49" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H648" s="49" t="s">
         <v>116</v>
@@ -20654,7 +20639,7 @@
     <row r="665" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A665" s="73"/>
       <c r="B665" s="48" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C665" s="75" t="s">
         <v>14</v>
@@ -20669,7 +20654,7 @@
         <v>15</v>
       </c>
       <c r="G665" s="49" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H665" s="49" t="s">
         <v>128</v>
@@ -21133,7 +21118,7 @@
     <row r="682" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A682" s="73"/>
       <c r="B682" s="48" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C682" s="75" t="s">
         <v>14</v>
@@ -21604,7 +21589,7 @@
     <row r="699" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A699" s="73"/>
       <c r="B699" s="48" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C699" s="75" t="s">
         <v>115</v>
@@ -21616,7 +21601,7 @@
         <v>14</v>
       </c>
       <c r="F699" s="75" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G699" s="49" t="s">
         <v>120</v>
@@ -21955,7 +21940,7 @@
         <v>75</v>
       </c>
       <c r="H710" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I710" s="61"/>
       <c r="J710" s="40"/>
@@ -22087,7 +22072,7 @@
     <row r="716" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A716" s="73"/>
       <c r="B716" s="48" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C716" s="75" t="s">
         <v>116</v>
@@ -22465,7 +22450,7 @@
         <v>0</v>
       </c>
       <c r="I728" s="113" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="J728" s="40"/>
       <c r="L728" s="40"/>
@@ -22570,7 +22555,7 @@
     <row r="733" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A733" s="73"/>
       <c r="B733" s="48" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C733" s="75" t="s">
         <v>12</v>
@@ -22588,7 +22573,7 @@
         <v>15</v>
       </c>
       <c r="H733" s="49" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I733" s="61"/>
       <c r="J733" s="40"/>
@@ -23057,7 +23042,7 @@
     <row r="750" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A750" s="73"/>
       <c r="B750" s="48" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C750" s="75" t="s">
         <v>14</v>
@@ -23075,7 +23060,7 @@
         <v>129</v>
       </c>
       <c r="H750" s="49" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I750" s="61"/>
       <c r="J750" s="40"/>
@@ -23540,7 +23525,7 @@
     <row r="767" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A767" s="73"/>
       <c r="B767" s="48" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C767" s="75" t="s">
         <v>116</v>
@@ -24019,7 +24004,7 @@
     <row r="784" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A784" s="73"/>
       <c r="B784" s="48" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C784" s="75" t="s">
         <v>103</v>
@@ -24034,7 +24019,7 @@
         <v>15</v>
       </c>
       <c r="G784" s="49" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H784" s="49" t="s">
         <v>12</v>
@@ -24508,7 +24493,7 @@
     <row r="801" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A801" s="73"/>
       <c r="B801" s="48" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C801" s="75" t="s">
         <v>12</v>
@@ -24523,7 +24508,7 @@
         <v>14</v>
       </c>
       <c r="G801" s="49" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="H801" s="49" t="s">
         <v>15</v>
@@ -24555,7 +24540,9 @@
       <c r="G802" s="5">
         <v>55</v>
       </c>
-      <c r="H802" s="5"/>
+      <c r="H802" s="5">
+        <v>76</v>
+      </c>
       <c r="I802" s="61"/>
       <c r="J802" s="40"/>
       <c r="L802" s="40"/>
@@ -24678,7 +24665,7 @@
       </c>
       <c r="H806" s="3">
         <f t="shared" si="134"/>
-        <v>59.8</v>
+        <v>75</v>
       </c>
       <c r="I806" s="61"/>
       <c r="J806" s="40"/>
@@ -24800,7 +24787,7 @@
       </c>
       <c r="H810" s="3">
         <f t="shared" si="135"/>
-        <v>67.900000000000006</v>
+        <v>71.7</v>
       </c>
       <c r="I810" s="61"/>
       <c r="J810" s="40"/>
@@ -24993,7 +24980,7 @@
     <row r="818" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A818" s="73"/>
       <c r="B818" s="48" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C818" s="75" t="s">
         <v>115</v>
@@ -25473,7 +25460,7 @@
     <row r="835" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A835" s="73"/>
       <c r="B835" s="48" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C835" s="75" t="s">
         <v>110</v>
@@ -25936,7 +25923,7 @@
         <v>12871</v>
       </c>
       <c r="B852" s="48" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C852" s="75" t="s">
         <v>116</v>
@@ -25951,7 +25938,7 @@
         <v>15</v>
       </c>
       <c r="G852" s="49" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H852" s="49" t="s">
         <v>128</v>
@@ -26415,7 +26402,7 @@
     <row r="869" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A869" s="73"/>
       <c r="B869" s="48" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C869" s="75" t="s">
         <v>131</v>
@@ -26898,7 +26885,7 @@
         <v>12880</v>
       </c>
       <c r="B886" s="48" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C886" s="75" t="s">
         <v>14</v>
@@ -27373,7 +27360,7 @@
     <row r="903" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A903" s="73"/>
       <c r="B903" s="48" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C903" s="75" t="s">
         <v>115</v>
@@ -27864,7 +27851,7 @@
     <row r="920" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A920" s="73"/>
       <c r="B920" s="48" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C920" s="75" t="s">
         <v>110</v>
@@ -27879,7 +27866,7 @@
         <v>15</v>
       </c>
       <c r="G920" s="49" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H920" s="49" t="s">
         <v>14</v>
@@ -28341,7 +28328,7 @@
     <row r="937" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A937" s="73"/>
       <c r="B937" s="48" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C937" s="75" t="s">
         <v>103</v>
@@ -28823,7 +28810,7 @@
     <row r="954" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A954" s="73"/>
       <c r="B954" s="48" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C954" s="75" t="s">
         <v>12</v>
@@ -29304,7 +29291,7 @@
     <row r="971" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A971" s="73"/>
       <c r="B971" s="48" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C971" s="75" t="s">
         <v>12</v>
@@ -29319,7 +29306,7 @@
         <v>14</v>
       </c>
       <c r="G971" s="49" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H971" s="49" t="s">
         <v>15</v>
@@ -29783,7 +29770,7 @@
         <v>12934</v>
       </c>
       <c r="B988" s="48" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C988" s="75" t="s">
         <v>15</v>
@@ -29798,7 +29785,7 @@
         <v>115</v>
       </c>
       <c r="G988" s="49" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H988" s="49" t="s">
         <v>129</v>
@@ -30254,7 +30241,7 @@
     <row r="1005" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1005" s="73"/>
       <c r="B1005" s="48" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C1005" s="75" t="s">
         <v>13</v>
@@ -30266,13 +30253,13 @@
         <v>115</v>
       </c>
       <c r="F1005" s="75" t="s">
-        <v>143</v>
+        <v>14</v>
       </c>
       <c r="G1005" s="49" t="s">
         <v>111</v>
       </c>
       <c r="H1005" s="49" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="I1005" s="61"/>
       <c r="J1005" s="40"/>
@@ -30727,7 +30714,7 @@
     <row r="1022" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1022" s="73"/>
       <c r="B1022" s="106" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C1022" s="75" t="s">
         <v>115</v>
@@ -31210,7 +31197,7 @@
     <row r="1039" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1039" s="73"/>
       <c r="B1039" s="48" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C1039" s="75" t="s">
         <v>14</v>
@@ -31222,7 +31209,7 @@
         <v>115</v>
       </c>
       <c r="F1039" s="75" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G1039" s="49" t="s">
         <v>13</v>
@@ -31686,13 +31673,13 @@
     <row r="1056" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1056" s="73"/>
       <c r="B1056" s="106" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C1056" s="75" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D1056" s="49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E1056" s="49" t="s">
         <v>13</v>
@@ -32173,7 +32160,7 @@
     <row r="1073" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1073" s="73"/>
       <c r="B1073" s="106" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C1073" s="75" t="s">
         <v>12</v>
@@ -32652,7 +32639,7 @@
     <row r="1090" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1090" s="73"/>
       <c r="B1090" s="74" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C1090" s="75" t="s">
         <v>112</v>
@@ -32763,7 +32750,7 @@
         <v>5</v>
       </c>
       <c r="I1093" s="113" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="J1093" s="40"/>
       <c r="L1093" s="40"/>
@@ -33133,7 +33120,7 @@
         <v>12776</v>
       </c>
       <c r="B1107" s="106" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C1107" s="75" t="s">
         <v>103</v>
@@ -33616,7 +33603,7 @@
     <row r="1124" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1124" s="73"/>
       <c r="B1124" s="106" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C1124" s="75" t="s">
         <v>126</v>
@@ -37178,14 +37165,14 @@
       <c r="B39" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="136" t="s">
+      <c r="C39" s="144" t="s">
         <v>18</v>
       </c>
-      <c r="D39" s="137"/>
-      <c r="E39" s="137"/>
-      <c r="F39" s="137"/>
-      <c r="G39" s="137"/>
-      <c r="H39" s="138"/>
+      <c r="D39" s="145"/>
+      <c r="E39" s="145"/>
+      <c r="F39" s="145"/>
+      <c r="G39" s="145"/>
+      <c r="H39" s="146"/>
       <c r="I39" s="4"/>
     </row>
     <row r="40" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -37241,14 +37228,14 @@
       <c r="B42" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C42" s="139" t="s">
+      <c r="C42" s="147" t="s">
         <v>18</v>
       </c>
-      <c r="D42" s="140"/>
-      <c r="E42" s="140"/>
-      <c r="F42" s="140"/>
-      <c r="G42" s="140"/>
-      <c r="H42" s="141"/>
+      <c r="D42" s="148"/>
+      <c r="E42" s="148"/>
+      <c r="F42" s="148"/>
+      <c r="G42" s="148"/>
+      <c r="H42" s="149"/>
       <c r="I42" s="4"/>
     </row>
     <row r="43" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated grade boundaries to M23
</commit_message>
<xml_diff>
--- a/Sample input.xlsx
+++ b/Sample input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Coding\PredictedGradeFlask\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Coding\predicted-grade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A5EE01-A5A5-41CE-A211-7E9C48359BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168B2F0D-EAA2-4635-B2E5-530B7F91B6DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Student Details" sheetId="1" r:id="rId1"/>
@@ -1769,7 +1769,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2114,23 +2114,15 @@
         <v>7</v>
       </c>
       <c r="C10" s="5">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D10" s="5">
-        <v>84</v>
-      </c>
-      <c r="E10" s="5">
-        <v>48</v>
-      </c>
-      <c r="F10" s="5">
-        <v>66</v>
-      </c>
-      <c r="G10" s="5">
-        <v>83</v>
-      </c>
-      <c r="H10" s="5">
-        <v>80</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
       <c r="I10" s="61"/>
       <c r="J10" s="40"/>
       <c r="L10" s="40"/>
@@ -2143,27 +2135,27 @@
       </c>
       <c r="C11" s="3">
         <f>0.05*C3+0.1*C4+C5+0.4*C6+C9+0.25*C10</f>
-        <v>142.14999999999998</v>
+        <v>142.64999999999998</v>
       </c>
       <c r="D11" s="3">
         <f>0.05*D3+0.1*D4+D5+0.4*D6+D9+0.25*D10</f>
-        <v>161.80000000000001</v>
+        <v>162.55000000000001</v>
       </c>
       <c r="E11" s="3">
         <f>0.05*E3+0.1*E4+E5+0.4*E6+E9+0.25*E10</f>
-        <v>134.80000000000001</v>
+        <v>122.8</v>
       </c>
       <c r="F11" s="3">
         <f>0.05*G3+0.1*F4+F5+0.4*F6+F9+0.25*F10</f>
-        <v>141.14999999999998</v>
+        <v>124.64999999999999</v>
       </c>
       <c r="G11" s="3">
         <f>0.05*G3+0.1*G4+G5+0.4*G6+G9+0.25*G10</f>
-        <v>154.19999999999999</v>
+        <v>133.44999999999999</v>
       </c>
       <c r="H11" s="3">
         <f>0.05*H3+0.1*H4+H5+0.4*H6+H9+0.25*H10</f>
-        <v>147.4</v>
+        <v>127.4</v>
       </c>
       <c r="I11" s="61"/>
       <c r="J11" s="40"/>
@@ -2282,24 +2274,24 @@
       </c>
       <c r="C16" s="99">
         <f>0.25*C10+0.25*C13+0.25*C14+C15</f>
-        <v>36</v>
+        <v>36.5</v>
       </c>
       <c r="D16" s="99">
         <f>0.25*D10+0.25*D13+0.25*D14+D15</f>
-        <v>75</v>
+        <v>75.75</v>
       </c>
       <c r="E16" s="99">
         <f>0.25*E10+0.25*E13+0.25*E14+E15</f>
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="F16" s="100">
         <f>0.25*F10+0.25*F13+0.25*F14+F15</f>
-        <v>62.75</v>
+        <v>46.25</v>
       </c>
       <c r="G16" s="99"/>
       <c r="H16" s="100">
         <f>0.25*H10+0.25*H13+0.25*H14+H15</f>
-        <v>72.25</v>
+        <v>52.25</v>
       </c>
       <c r="I16" s="92"/>
       <c r="J16" s="40"/>

</xml_diff>